<commit_message>
v0.1.6. Copying template objects was implemented
</commit_message>
<xml_diff>
--- a/templates/Base.xlsx
+++ b/templates/Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\Projects\ResponseAnalyzer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E13CCA-2BD4-479B-83BD-61AAC8A6B3BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CA48AE-B0C5-40A3-90BE-D8E7F0A6A6E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A8E955EB-F13F-4C65-9C3C-6EA905D67102}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{A8E955EB-F13F-4C65-9C3C-6EA905D67102}"/>
   </bookViews>
   <sheets>
     <sheet name="АЧХ" sheetId="2" r:id="rId1"/>
@@ -5958,7 +5958,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Фюзеляж">
+        <xdr:cNvPr id="4" name="Фюзеляж-Ф">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE6E940-8D78-463E-85E3-6CEAF382CB22}"/>
@@ -5996,7 +5996,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Крыло">
+        <xdr:cNvPr id="5" name="Крыло-Ф">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{802016C6-EA80-4B88-876A-0B160F3C9577}"/>
@@ -6524,7 +6524,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Стабилизатор">
+        <xdr:cNvPr id="10" name="Стабилизатор-Ф">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AB84C13-E786-4785-83C8-1473E08B5D0E}"/>
@@ -6789,7 +6789,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Киль">
+        <xdr:cNvPr id="13" name="Киль-Ф">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CB2A726-ACD3-491C-B36D-BD5A0AB0A226}"/>
@@ -7324,8 +7324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3406B6-B537-451D-BC5F-1BF62CD9F844}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7344,8 +7344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A104BF4C-683E-43E8-A927-D03CE3B9A284}">
   <dimension ref="A1:AI627"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.1.8. Binary templates were implemented
</commit_message>
<xml_diff>
--- a/templates/Base.xlsx
+++ b/templates/Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\Projects\ResponseAnalyzer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD69623F-1012-4EE8-A5DD-9046C8A426F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C7A5F7-E051-4D7A-9DA0-C5BD3D350233}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{A8E955EB-F13F-4C65-9C3C-6EA905D67102}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="15">
   <si>
     <t>Мнимая</t>
   </si>
@@ -8638,7 +8638,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8704,8 +8704,8 @@
       <c r="D3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>12</v>
+      <c r="E3" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>12</v>
@@ -8726,7 +8726,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>7</v>
@@ -8746,8 +8746,8 @@
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>14</v>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>14</v>
@@ -8767,8 +8767,8 @@
       <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>8</v>
+      <c r="E6" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>8</v>
@@ -8789,7 +8789,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>9</v>
@@ -8811,8 +8811,8 @@
       <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>11</v>
+      <c r="E8" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>11</v>
@@ -8832,8 +8832,8 @@
       <c r="D9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>10</v>
+      <c r="E9" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>10</v>
@@ -8853,9 +8853,7 @@
       <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="E10" s="6"/>
       <c r="F10" s="9" t="s">
         <v>5</v>
       </c>
@@ -8868,7 +8866,7 @@
       <c r="D11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="9"/>
+      <c r="E11" s="6"/>
       <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
@@ -8878,7 +8876,7 @@
       <c r="D12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
@@ -8888,7 +8886,7 @@
       <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
@@ -8898,7 +8896,7 @@
       <c r="D14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="9"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
@@ -8908,7 +8906,7 @@
       <c r="D15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="9"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
@@ -8918,7 +8916,7 @@
       <c r="D16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="9"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
@@ -8928,7 +8926,7 @@
       <c r="D17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="9"/>
+      <c r="E17" s="5"/>
       <c r="F17" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.2.2.3. Implement line styles
</commit_message>
<xml_diff>
--- a/templates/Base.xlsx
+++ b/templates/Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\Projects\ResponseAnalyzer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9253AB-FB8D-4FAD-B896-D8EFD6D8C0E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0FEE00-FEAD-419A-85EF-1D57986F51B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{A8E955EB-F13F-4C65-9C3C-6EA905D67102}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="5" xr2:uid="{A8E955EB-F13F-4C65-9C3C-6EA905D67102}"/>
   </bookViews>
   <sheets>
     <sheet name="АЧХ" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Вращение" sheetId="4" r:id="rId3"/>
     <sheet name="f(A)" sheetId="5" r:id="rId4"/>
     <sheet name="Markers" sheetId="3" r:id="rId5"/>
+    <sheet name="Lines" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="19">
   <si>
     <t>Мнимая</t>
   </si>
@@ -74,6 +75,18 @@
   </si>
   <si>
     <t>●</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>x━</t>
+  </si>
+  <si>
+    <t>x--</t>
+  </si>
+  <si>
+    <t>━</t>
   </si>
 </sst>
 </file>
@@ -10833,8 +10846,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6743700" y="723900"/>
-          <a:ext cx="1536701" cy="1360489"/>
+          <a:off x="6911340" y="723900"/>
+          <a:ext cx="1567181" cy="1360489"/>
           <a:chOff x="7370763" y="1735136"/>
           <a:chExt cx="1536701" cy="1331914"/>
         </a:xfrm>
@@ -14714,9 +14727,9 @@
       <selection activeCell="L53" sqref="K53:L53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14732,9 +14745,9 @@
       <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14750,9 +14763,9 @@
       <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -14764,7 +14777,7 @@
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -14776,7 +14789,7 @@
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -14788,7 +14801,7 @@
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -14800,7 +14813,7 @@
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -14812,7 +14825,7 @@
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -14824,7 +14837,7 @@
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -14836,7 +14849,7 @@
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -14848,7 +14861,7 @@
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -14860,7 +14873,7 @@
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -14872,7 +14885,7 @@
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -14884,7 +14897,7 @@
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -14896,7 +14909,7 @@
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -14908,7 +14921,7 @@
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -14920,7 +14933,7 @@
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -14932,7 +14945,7 @@
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -14944,7 +14957,7 @@
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -14956,7 +14969,7 @@
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -14968,7 +14981,7 @@
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -14980,7 +14993,7 @@
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -14992,7 +15005,7 @@
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -15004,7 +15017,7 @@
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -15016,7 +15029,7 @@
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -15028,7 +15041,7 @@
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -15040,7 +15053,7 @@
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -15052,7 +15065,7 @@
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -15064,7 +15077,7 @@
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -15076,7 +15089,7 @@
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -15088,7 +15101,7 @@
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -15100,7 +15113,7 @@
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -15112,7 +15125,7 @@
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -15124,7 +15137,7 @@
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -15136,7 +15149,7 @@
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -15148,7 +15161,7 @@
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -15160,7 +15173,7 @@
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -15172,7 +15185,7 @@
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -15184,7 +15197,7 @@
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -15196,7 +15209,7 @@
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -15208,7 +15221,7 @@
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -15220,7 +15233,7 @@
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -15232,7 +15245,7 @@
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="14"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
@@ -15244,7 +15257,7 @@
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="14"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -15256,7 +15269,7 @@
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="14"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -15268,7 +15281,7 @@
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -15280,7 +15293,7 @@
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -15292,7 +15305,7 @@
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -15304,7 +15317,7 @@
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="14"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
@@ -15316,7 +15329,7 @@
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="14"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -15328,7 +15341,7 @@
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="14"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
@@ -15340,7 +15353,7 @@
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="14"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
@@ -15352,7 +15365,7 @@
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="14"/>
       <c r="B51" s="14"/>
       <c r="C51" s="14"/>
@@ -15364,7 +15377,7 @@
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
@@ -15376,7 +15389,7 @@
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="14"/>
       <c r="B53" s="14"/>
       <c r="C53" s="14"/>
@@ -15388,7 +15401,7 @@
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="14"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
@@ -15400,7 +15413,7 @@
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
@@ -15422,13 +15435,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3823255-2A8F-4FC4-847E-C4C254012FBF}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -15439,7 +15452,7 @@
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -15450,7 +15463,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -15461,7 +15474,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -15472,7 +15485,7 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -15483,7 +15496,7 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -15494,7 +15507,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -15505,7 +15518,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -15516,7 +15529,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
@@ -15527,7 +15540,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -15538,7 +15551,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -15549,7 +15562,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -15560,7 +15573,7 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -15571,7 +15584,7 @@
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -15582,7 +15595,7 @@
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -15593,7 +15606,7 @@
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -15604,7 +15617,7 @@
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -15615,7 +15628,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -15626,7 +15639,7 @@
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -15637,7 +15650,7 @@
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -15648,7 +15661,7 @@
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -15659,7 +15672,7 @@
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -15670,7 +15683,7 @@
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -15681,7 +15694,7 @@
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -15692,7 +15705,7 @@
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -15703,7 +15716,7 @@
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -15714,7 +15727,7 @@
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -15725,7 +15738,7 @@
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -15736,7 +15749,7 @@
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -15747,7 +15760,7 @@
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -15758,7 +15771,7 @@
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -15780,19 +15793,19 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F18" sqref="A1:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="15.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="3" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" style="3"/>
-    <col min="11" max="11" width="9.140625" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="5" width="15.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="3" customWidth="1"/>
+    <col min="7" max="10" width="9.109375" style="3"/>
+    <col min="11" max="11" width="9.109375" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -15812,7 +15825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -15833,7 +15846,7 @@
       </c>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -15854,7 +15867,7 @@
       </c>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -15875,7 +15888,7 @@
       </c>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.4">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
@@ -15896,7 +15909,7 @@
       </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -15917,7 +15930,7 @@
       </c>
       <c r="K6" s="11"/>
     </row>
-    <row r="7" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -15940,7 +15953,7 @@
       <c r="K7" s="10"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="19.8" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
@@ -15961,7 +15974,7 @@
       </c>
       <c r="K8" s="12"/>
     </row>
-    <row r="9" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -15982,7 +15995,7 @@
       </c>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="19.8" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>5</v>
       </c>
@@ -16001,7 +16014,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="19.8" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -16011,7 +16024,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="19.8" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -16021,7 +16034,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="19.8" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -16031,7 +16044,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -16041,7 +16054,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -16051,7 +16064,7 @@
       <c r="E15" s="7"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:15" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="19.8" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -16061,7 +16074,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -16075,4 +16088,208 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222B3248-D0DD-497C-B416-49A4AA0D08AD}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
v0.2.2.4. Create references to signals in case of FRF
</commit_message>
<xml_diff>
--- a/templates/Base.xlsx
+++ b/templates/Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Library\Projects\ResponseAnalyzer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0FEE00-FEAD-419A-85EF-1D57986F51B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0F437B-3E1E-4F19-AB05-9CCDF8DEB7D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="5" xr2:uid="{A8E955EB-F13F-4C65-9C3C-6EA905D67102}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="19">
   <si>
     <t>Мнимая</t>
   </si>
@@ -77,16 +77,16 @@
     <t>●</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>x━</t>
   </si>
   <si>
-    <t>x--</t>
+    <t>━</t>
   </si>
   <si>
-    <t>━</t>
+    <t>Действительная-ВР</t>
+  </si>
+  <si>
+    <t>Мнимая-ВР</t>
   </si>
 </sst>
 </file>
@@ -211,7 +211,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
@@ -249,6 +249,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -798,8 +801,6 @@
         <c:axId val="169085760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="24"/>
-          <c:min val="21"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -837,15 +838,11 @@
         <c:crossAx val="169086336"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.5"/>
-        <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="169086336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="10"/>
-          <c:min val="-10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -883,8 +880,6 @@
         <c:crossAx val="169085760"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5"/>
-        <c:minorUnit val="5"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1536,8 +1531,6 @@
         <c:axId val="169089792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="24"/>
-          <c:min val="21"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1575,15 +1568,11 @@
         <c:crossAx val="181626560"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.5"/>
-        <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="181626560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="10"/>
-          <c:min val="-10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1621,8 +1610,6 @@
         <c:crossAx val="169089792"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5"/>
-        <c:minorUnit val="5"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -2120,8 +2107,6 @@
         <c:axId val="362330304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="6"/>
-          <c:min val="-6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -2168,8 +2153,6 @@
         <c:crossAx val="362329728"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="6"/>
-        <c:minorUnit val="3"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -3245,8 +3228,6 @@
         <c:axId val="362333888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="12"/>
-          <c:min val="-18"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3293,8 +3274,6 @@
         <c:crossAx val="362333312"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="6"/>
-        <c:minorUnit val="6"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -3725,8 +3704,6 @@
         <c:axId val="362343808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="6"/>
-          <c:min val="-6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3773,8 +3750,6 @@
         <c:crossAx val="362343232"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="6"/>
-        <c:minorUnit val="3"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -4072,8 +4047,6 @@
         <c:axId val="362346688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="6"/>
-          <c:min val="-6"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4120,8 +4093,6 @@
         <c:crossAx val="362347264"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="6"/>
-        <c:minorUnit val="3"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="362347264"/>
@@ -5701,8 +5672,6 @@
         <c:axId val="262404864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="35"/>
-          <c:min val="22"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -5740,7 +5709,6 @@
         <c:crossAx val="262405440"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:minorUnit val="2"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="262405440"/>
@@ -5783,7 +5751,6 @@
         <c:crossAx val="262404864"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:minorUnit val="10"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -7387,8 +7354,6 @@
         <c:axId val="175810240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="35"/>
-          <c:min val="22"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -7426,7 +7391,6 @@
         <c:crossAx val="175810816"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:minorUnit val="2"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="175810816"/>
@@ -7469,8 +7433,6 @@
         <c:crossAx val="175810240"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="10"/>
-        <c:minorUnit val="10"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -7799,13 +7761,11 @@
         <c:crossAx val="175814272"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:minorUnit val="10"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="175814272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="24"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -7843,7 +7803,6 @@
         <c:crossAx val="175813696"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
-        <c:minorUnit val="1"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -14724,7 +14683,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L53" sqref="K53:L53"/>
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14741,8 +14700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A104BF4C-683E-43E8-A927-D03CE3B9A284}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14759,8 +14718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C9E1E0D-5F10-4C4C-8945-2EBD06D66BC3}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15436,7 +15395,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U29" sqref="U29"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16092,23 +16051,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222B3248-D0DD-497C-B416-49A4AA0D08AD}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -16127,128 +16089,128 @@
       <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="H2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="5"/>
+    <row r="3" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+    <row r="4" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
     </row>
-    <row r="5" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
+    <row r="5" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
+    <row r="6" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+    <row r="7" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
     </row>
-    <row r="8" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="5"/>
+    <row r="9" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -16256,7 +16218,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:6" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -16264,29 +16226,21 @@
       <c r="E15" s="7"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" ht="19.8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="19.8" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
       <c r="F17" s="9"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>